<commit_message>
fix: deleted one register in "evaluate 2.xlsx" file
</commit_message>
<xml_diff>
--- a/assets/default_corpus/model_type_one/evaluate 2.xlsx
+++ b/assets/default_corpus/model_type_one/evaluate 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CUJAE\DeepLearning\Software Required\Parser Proyect\assets\default_corpus\model_type_one\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F8C247-2F0A-4038-8C9D-3303992F1906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D3233B-F50A-47FF-A92E-57B1FA5D4036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE3A1A6B-7415-49B6-8F8D-6A02B855C26B}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{CE3A1A6B-7415-49B6-8F8D-6A02B855C26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Direcciones Reales</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Ave Entrada E / Ave de los Ocujes y Ave  de la Ceiba Edificio 2 APTO 5 Reparto Santa Catalina,CERRO,La Habana</t>
-  </si>
-  <si>
-    <t>Calle Camilo Cienfuegos, Finca San Juan  # 91, Poblado Bacuranao,GUANABACOA,La Habana</t>
   </si>
   <si>
     <t>Aliados e/ Pasaje D y Central, San Miguel del Padrón, La Habana</t>
@@ -235,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,7 +241,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,9 +556,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04EBE9F-E917-492C-AF6B-0ED5EB213D61}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -667,7 +663,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
@@ -711,8 +707,8 @@
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>45</v>
+      <c r="A28" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
@@ -727,7 +723,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -737,7 +733,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -757,7 +753,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -791,18 +787,18 @@
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+      <c r="A44" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
@@ -818,11 +814,6 @@
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>